<commit_message>
First draft of results and conclusion
</commit_message>
<xml_diff>
--- a/Presentation/experimental-results.xlsx
+++ b/Presentation/experimental-results.xlsx
@@ -167,27 +167,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +491,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -500,37 +502,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -538,17 +540,17 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="5">
         <v>23.6</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="6">
         <f>I4</f>
         <v>2</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="9">
         <v>36.200000000000003</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="6">
         <f>I3</f>
         <v>1</v>
       </c>
@@ -570,17 +572,17 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="5">
         <v>16.100000000000001</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="6">
         <f>I4</f>
         <v>2</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="9">
         <v>30.4</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <f>I3</f>
         <v>1</v>
       </c>
@@ -599,17 +601,17 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="15">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="11">
         <v>20.170000000000002</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f>I5</f>
         <v>3</v>
       </c>
@@ -624,10 +626,10 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="9"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="1">
         <v>17.7</v>
       </c>

</xml_diff>